<commit_message>
Add ODK Tables list/detail views for ingrow/mort.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/mortality/forms/mortality/mortality.xlsx
+++ b/odk_app/config/tables/mortality/forms/mortality/mortality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\dev\classes\capstone\app-designer-2.1.6\app\config\tables\mortality\forms\mortality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\mortality\forms\mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0AC587-3D88-43EE-98C1-A30A665D624C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5D4747-E1CE-4DE8-B7AD-2241A3E3E8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26850" yWindow="7800" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="264">
   <si>
     <t>clause</t>
   </si>
@@ -802,6 +802,24 @@
   </si>
   <si>
     <t>Velvet top butt rot (Phaeolus schweinitzii)</t>
+  </si>
+  <si>
+    <t>Support percentage</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>Tag</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A8133D-3FC4-43E4-B3AE-EB32F6785EEA}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1293,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,52 +1354,52 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
+        <v>259</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>260</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
+        <v>259</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>262</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>15</v>
+        <v>181</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>15</v>
+        <v>181</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,10 +1407,10 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,10 +1418,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>187</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1411,38 +1429,32 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>188</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>181</v>
-      </c>
-      <c r="D10" t="s">
-        <v>195</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="F10" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D11" t="s">
-        <v>195</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F11" t="s">
-        <v>201</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1453,10 +1465,10 @@
         <v>195</v>
       </c>
       <c r="E12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,10 +1479,10 @@
         <v>195</v>
       </c>
       <c r="E13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1478,13 +1490,13 @@
         <v>181</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E14" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,57 +1504,57 @@
         <v>181</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E15" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>17</v>
+        <v>181</v>
+      </c>
+      <c r="D16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" t="s">
+        <v>192</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>17</v>
+        <v>181</v>
+      </c>
+      <c r="D17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" t="s">
+        <v>193</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" t="s">
-        <v>248</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" t="s">
-        <v>248</v>
-      </c>
-      <c r="E19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1553,25 +1565,53 @@
         <v>248</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" t="s">
+        <v>248</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>52</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>53</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>